<commit_message>
updating results file and rounding precision for sp conductance for instrument checks, fix #19
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleResults.xlsx
+++ b/inst/extdata/ExampleResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2419E6A6-3D7C-4A0E-A765-0A376B36FE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA845B59-DFA3-44BD-B103-00ACC15942F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16025" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16083" uniqueCount="139">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -486,6 +486,15 @@
   </si>
   <si>
     <t>R2546-13</t>
+  </si>
+  <si>
+    <t>pH-6-15-5</t>
+  </si>
+  <si>
+    <t>pH-6-16-5</t>
+  </si>
+  <si>
+    <t>pH-6-17-5</t>
   </si>
 </sst>
 </file>
@@ -909,13 +918,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N2639"/>
+  <dimension ref="A1:N2653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2599" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E957" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2612" sqref="L2612"/>
+      <selection pane="bottomRight" activeCell="I968" sqref="I968"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31851,10 +31860,13 @@
         <v>90</v>
       </c>
       <c r="I965">
-        <v>886</v>
+        <v>138</v>
       </c>
       <c r="J965" t="s">
         <v>98</v>
+      </c>
+      <c r="L965">
+        <v>148</v>
       </c>
       <c r="M965" t="s">
         <v>13</v>
@@ -31883,10 +31895,13 @@
         <v>90</v>
       </c>
       <c r="I966">
-        <v>954</v>
+        <v>138</v>
       </c>
       <c r="J966" t="s">
         <v>98</v>
+      </c>
+      <c r="L966">
+        <v>149</v>
       </c>
       <c r="M966" t="s">
         <v>13</v>
@@ -31915,10 +31930,13 @@
         <v>90</v>
       </c>
       <c r="I967">
-        <v>963</v>
+        <v>138.5</v>
       </c>
       <c r="J967" t="s">
         <v>98</v>
+      </c>
+      <c r="L967">
+        <v>149.6</v>
       </c>
       <c r="M967" t="s">
         <v>13</v>
@@ -82098,7 +82116,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2529" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2529" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2529" t="s">
         <v>43</v>
       </c>
@@ -82130,7 +82148,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="2530" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2530" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2530" t="s">
         <v>43</v>
       </c>
@@ -82162,7 +82180,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="2531" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2531" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2531" t="s">
         <v>26</v>
       </c>
@@ -82191,7 +82209,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2532" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2532" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2532" t="s">
         <v>14</v>
       </c>
@@ -82220,7 +82238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2533" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2533" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2533" t="s">
         <v>22</v>
       </c>
@@ -82249,7 +82267,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2534" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2534" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2534" t="s">
         <v>30</v>
       </c>
@@ -82278,7 +82296,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2535" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2535" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2535" t="s">
         <v>31</v>
       </c>
@@ -82307,7 +82325,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2536" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2536" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2536" t="s">
         <v>72</v>
       </c>
@@ -82330,7 +82348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2537" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2537" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2537" t="s">
         <v>72</v>
       </c>
@@ -82353,7 +82371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2538" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2538" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2538" t="s">
         <v>72</v>
       </c>
@@ -82376,15 +82394,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2539" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2539" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2539" t="s">
         <v>72</v>
       </c>
       <c r="C2539" s="4">
-        <v>44388</v>
+        <v>44242</v>
       </c>
       <c r="D2539" s="5">
-        <v>0.30208333333333298</v>
+        <v>0.28888888888888897</v>
       </c>
       <c r="H2539" t="s">
         <v>87</v>
@@ -82395,34 +82413,40 @@
       <c r="J2539" t="s">
         <v>96</v>
       </c>
+      <c r="K2539">
+        <v>0.2</v>
+      </c>
       <c r="M2539" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2540" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2540" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2540" t="s">
         <v>72</v>
       </c>
       <c r="C2540" s="4">
-        <v>44388</v>
+        <v>44243</v>
       </c>
       <c r="D2540" s="5">
-        <v>0.30902777777777801</v>
+        <v>0.28888888888888897</v>
       </c>
       <c r="H2540" t="s">
         <v>87</v>
       </c>
       <c r="I2540">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="J2540" t="s">
         <v>96</v>
       </c>
+      <c r="K2540">
+        <v>0.02</v>
+      </c>
       <c r="M2540" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2541" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2541" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2541" t="s">
         <v>72</v>
       </c>
@@ -82430,7 +82454,7 @@
         <v>44388</v>
       </c>
       <c r="D2541" s="5">
-        <v>0.32291666666666702</v>
+        <v>0.30208333333333298</v>
       </c>
       <c r="H2541" t="s">
         <v>87</v>
@@ -82445,7 +82469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2542" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2542" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2542" t="s">
         <v>72</v>
       </c>
@@ -82453,13 +82477,13 @@
         <v>44388</v>
       </c>
       <c r="D2542" s="5">
-        <v>0.343055555555556</v>
+        <v>0.30902777777777801</v>
       </c>
       <c r="H2542" t="s">
         <v>87</v>
       </c>
-      <c r="I2542" t="s">
-        <v>74</v>
+      <c r="I2542">
+        <v>0.11</v>
       </c>
       <c r="J2542" t="s">
         <v>96</v>
@@ -82468,15 +82492,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2543" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2543" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2543" t="s">
         <v>72</v>
       </c>
       <c r="C2543" s="4">
-        <v>44360</v>
+        <v>44388</v>
+      </c>
+      <c r="D2543" s="5">
+        <v>0.32291666666666702</v>
       </c>
       <c r="H2543" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="I2543" t="s">
         <v>74</v>
@@ -82484,28 +82511,31 @@
       <c r="J2543" t="s">
         <v>96</v>
       </c>
-      <c r="N2543" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2544" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2543" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2544" t="s">
         <v>72</v>
       </c>
       <c r="C2544" s="4">
-        <v>44360</v>
+        <v>44388</v>
+      </c>
+      <c r="D2544" s="5">
+        <v>0.343055555555556</v>
       </c>
       <c r="H2544" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2544">
-        <v>0.1</v>
+        <v>87</v>
+      </c>
+      <c r="I2544" t="s">
+        <v>74</v>
       </c>
       <c r="J2544" t="s">
         <v>96</v>
       </c>
-      <c r="N2544" t="s">
-        <v>117</v>
+      <c r="M2544" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2545" spans="2:14" x14ac:dyDescent="0.25">
@@ -82525,7 +82555,7 @@
         <v>96</v>
       </c>
       <c r="N2545" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2546" spans="2:14" x14ac:dyDescent="0.25">
@@ -82538,14 +82568,14 @@
       <c r="H2546" t="s">
         <v>68</v>
       </c>
-      <c r="I2546" t="s">
-        <v>74</v>
+      <c r="I2546">
+        <v>0.1</v>
       </c>
       <c r="J2546" t="s">
         <v>96</v>
       </c>
       <c r="N2546" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2547" spans="2:14" x14ac:dyDescent="0.25">
@@ -82558,14 +82588,14 @@
       <c r="H2547" t="s">
         <v>68</v>
       </c>
-      <c r="I2547">
-        <v>0.02</v>
+      <c r="I2547" t="s">
+        <v>74</v>
       </c>
       <c r="J2547" t="s">
         <v>96</v>
       </c>
       <c r="N2547" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2548" spans="2:14" x14ac:dyDescent="0.25">
@@ -82585,7 +82615,7 @@
         <v>96</v>
       </c>
       <c r="N2548" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2549" spans="2:14" x14ac:dyDescent="0.25">
@@ -82598,14 +82628,14 @@
       <c r="H2549" t="s">
         <v>68</v>
       </c>
-      <c r="I2549" t="s">
-        <v>74</v>
+      <c r="I2549">
+        <v>0.02</v>
       </c>
       <c r="J2549" t="s">
         <v>96</v>
       </c>
       <c r="N2549" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2550" spans="2:14" x14ac:dyDescent="0.25">
@@ -82618,14 +82648,14 @@
       <c r="H2550" t="s">
         <v>68</v>
       </c>
-      <c r="I2550">
-        <v>0.03</v>
+      <c r="I2550" t="s">
+        <v>74</v>
       </c>
       <c r="J2550" t="s">
         <v>96</v>
       </c>
       <c r="N2550" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2551" spans="2:14" x14ac:dyDescent="0.25">
@@ -82633,16 +82663,19 @@
         <v>72</v>
       </c>
       <c r="C2551" s="4">
-        <v>44297</v>
+        <v>44360</v>
       </c>
       <c r="H2551" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2551">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="I2551" t="s">
+        <v>74</v>
       </c>
       <c r="J2551" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="N2551" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="2552" spans="2:14" x14ac:dyDescent="0.25">
@@ -82650,16 +82683,19 @@
         <v>72</v>
       </c>
       <c r="C2552" s="4">
-        <v>44297</v>
+        <v>44360</v>
       </c>
       <c r="H2552" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="I2552">
-        <v>5</v>
+        <v>0.03</v>
       </c>
       <c r="J2552" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="N2552" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2553" spans="2:14" x14ac:dyDescent="0.25">
@@ -82673,7 +82709,7 @@
         <v>90</v>
       </c>
       <c r="I2553">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="J2553" t="s">
         <v>98</v>
@@ -82684,19 +82720,16 @@
         <v>72</v>
       </c>
       <c r="C2554" s="4">
-        <v>44298</v>
+        <v>44297</v>
       </c>
       <c r="H2554" t="s">
         <v>90</v>
       </c>
-      <c r="I2554" t="s">
-        <v>74</v>
+      <c r="I2554">
+        <v>5</v>
       </c>
       <c r="J2554" t="s">
         <v>98</v>
-      </c>
-      <c r="K2554">
-        <v>50</v>
       </c>
     </row>
     <row r="2555" spans="2:14" x14ac:dyDescent="0.25">
@@ -82704,13 +82737,13 @@
         <v>72</v>
       </c>
       <c r="C2555" s="4">
-        <v>44299</v>
+        <v>44297</v>
       </c>
       <c r="H2555" t="s">
         <v>90</v>
       </c>
-      <c r="I2555" t="s">
-        <v>74</v>
+      <c r="I2555">
+        <v>25</v>
       </c>
       <c r="J2555" t="s">
         <v>98</v>
@@ -82718,54 +82751,39 @@
     </row>
     <row r="2556" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2556" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2556" s="4">
-        <v>44452</v>
+        <v>44298</v>
       </c>
       <c r="H2556" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2556">
-        <v>128</v>
+        <v>90</v>
+      </c>
+      <c r="I2556" t="s">
+        <v>74</v>
       </c>
       <c r="J2556" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2556">
-        <v>150</v>
-      </c>
-      <c r="M2556" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2556" t="s">
-        <v>130</v>
+        <v>98</v>
+      </c>
+      <c r="K2556">
+        <v>50</v>
       </c>
     </row>
     <row r="2557" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2557" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2557" s="4">
-        <v>44389</v>
+        <v>44299</v>
       </c>
       <c r="H2557" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2557">
-        <v>40</v>
+        <v>90</v>
+      </c>
+      <c r="I2557" t="s">
+        <v>74</v>
       </c>
       <c r="J2557" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2557">
-        <v>10</v>
-      </c>
-      <c r="M2557" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2557" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2558" spans="2:14" x14ac:dyDescent="0.25">
@@ -82773,25 +82791,25 @@
         <v>71</v>
       </c>
       <c r="C2558" s="4">
-        <v>44389</v>
+        <v>44452</v>
       </c>
       <c r="H2558" t="s">
         <v>92</v>
       </c>
       <c r="I2558">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="J2558" t="s">
         <v>100</v>
       </c>
       <c r="L2558">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="M2558" t="s">
         <v>13</v>
       </c>
       <c r="N2558" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2559" spans="2:14" x14ac:dyDescent="0.25">
@@ -82799,25 +82817,25 @@
         <v>71</v>
       </c>
       <c r="C2559" s="4">
-        <v>44396</v>
+        <v>44389</v>
       </c>
       <c r="H2559" t="s">
         <v>92</v>
       </c>
       <c r="I2559">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="J2559" t="s">
         <v>100</v>
       </c>
       <c r="L2559">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="M2559" t="s">
         <v>13</v>
       </c>
       <c r="N2559" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2560" spans="2:14" x14ac:dyDescent="0.25">
@@ -82825,25 +82843,25 @@
         <v>71</v>
       </c>
       <c r="C2560" s="4">
-        <v>44396</v>
+        <v>44389</v>
       </c>
       <c r="H2560" t="s">
         <v>92</v>
       </c>
       <c r="I2560">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="J2560" t="s">
         <v>100</v>
       </c>
       <c r="L2560">
-        <v>250</v>
+        <v>37</v>
       </c>
       <c r="M2560" t="s">
         <v>13</v>
       </c>
       <c r="N2560" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2561" spans="2:14" x14ac:dyDescent="0.25">
@@ -82857,7 +82875,7 @@
         <v>92</v>
       </c>
       <c r="I2561">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="J2561" t="s">
         <v>100</v>
@@ -82869,7 +82887,7 @@
         <v>13</v>
       </c>
       <c r="N2561" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2562" spans="2:14" x14ac:dyDescent="0.25">
@@ -82877,28 +82895,25 @@
         <v>71</v>
       </c>
       <c r="C2562" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2562" s="5">
-        <v>0.27083333333333298</v>
+        <v>44396</v>
       </c>
       <c r="H2562" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="I2562">
-        <v>0.8</v>
+        <v>100</v>
       </c>
       <c r="J2562" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L2562">
-        <v>0.9</v>
+        <v>250</v>
       </c>
       <c r="M2562" t="s">
         <v>13</v>
       </c>
       <c r="N2562" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2563" spans="2:14" x14ac:dyDescent="0.25">
@@ -82906,28 +82921,25 @@
         <v>71</v>
       </c>
       <c r="C2563" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2563" s="5">
-        <v>0.27777777777777801</v>
+        <v>44396</v>
       </c>
       <c r="H2563" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="I2563">
-        <v>0.3</v>
+        <v>800</v>
       </c>
       <c r="J2563" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L2563">
-        <v>0.3</v>
+        <v>400</v>
       </c>
       <c r="M2563" t="s">
         <v>13</v>
       </c>
       <c r="N2563" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2564" spans="2:14" x14ac:dyDescent="0.25">
@@ -82938,25 +82950,25 @@
         <v>44332</v>
       </c>
       <c r="D2564" s="5">
-        <v>0.28819444444444398</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="H2564" t="s">
         <v>86</v>
       </c>
       <c r="I2564">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="J2564" t="s">
         <v>96</v>
       </c>
       <c r="L2564">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="M2564" t="s">
         <v>13</v>
       </c>
       <c r="N2564" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2565" spans="2:14" x14ac:dyDescent="0.25">
@@ -82967,25 +82979,25 @@
         <v>44332</v>
       </c>
       <c r="D2565" s="5">
-        <v>0.30208333333333298</v>
+        <v>0.27777777777777801</v>
       </c>
       <c r="H2565" t="s">
         <v>86</v>
       </c>
       <c r="I2565">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="J2565" t="s">
         <v>96</v>
       </c>
       <c r="L2565">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="M2565" t="s">
         <v>13</v>
       </c>
       <c r="N2565" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2566" spans="2:14" x14ac:dyDescent="0.25">
@@ -82996,13 +83008,13 @@
         <v>44332</v>
       </c>
       <c r="D2566" s="5">
-        <v>0.31944444444444398</v>
+        <v>0.28819444444444398</v>
       </c>
       <c r="H2566" t="s">
         <v>86</v>
       </c>
       <c r="I2566">
-        <v>0.12</v>
+        <v>0.45</v>
       </c>
       <c r="J2566" t="s">
         <v>96</v>
@@ -83014,7 +83026,7 @@
         <v>13</v>
       </c>
       <c r="N2566" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2567" spans="2:14" x14ac:dyDescent="0.25">
@@ -83025,25 +83037,25 @@
         <v>44332</v>
       </c>
       <c r="D2567" s="5">
-        <v>0.32638888888888901</v>
+        <v>0.30208333333333298</v>
       </c>
       <c r="H2567" t="s">
         <v>86</v>
       </c>
       <c r="I2567">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
       <c r="J2567" t="s">
         <v>96</v>
       </c>
       <c r="L2567">
-        <v>0.21</v>
+        <v>0.82</v>
       </c>
       <c r="M2567" t="s">
         <v>13</v>
       </c>
       <c r="N2567" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2568" spans="2:14" x14ac:dyDescent="0.25">
@@ -83054,25 +83066,25 @@
         <v>44332</v>
       </c>
       <c r="D2568" s="5">
-        <v>0.33333333333333298</v>
+        <v>0.31944444444444398</v>
       </c>
       <c r="H2568" t="s">
         <v>86</v>
       </c>
       <c r="I2568">
-        <v>0.45</v>
+        <v>0.12</v>
       </c>
       <c r="J2568" t="s">
         <v>96</v>
       </c>
       <c r="L2568">
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
       <c r="M2568" t="s">
         <v>13</v>
       </c>
       <c r="N2568" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2569" spans="2:14" x14ac:dyDescent="0.25">
@@ -83083,25 +83095,25 @@
         <v>44332</v>
       </c>
       <c r="D2569" s="5">
-        <v>0.34375</v>
+        <v>0.32638888888888901</v>
       </c>
       <c r="H2569" t="s">
         <v>86</v>
       </c>
       <c r="I2569">
-        <v>0.08</v>
+        <v>0.34</v>
       </c>
       <c r="J2569" t="s">
         <v>96</v>
       </c>
       <c r="L2569">
-        <v>0.08</v>
+        <v>0.21</v>
       </c>
       <c r="M2569" t="s">
         <v>13</v>
       </c>
       <c r="N2569" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2570" spans="2:14" x14ac:dyDescent="0.25">
@@ -83109,7 +83121,7 @@
         <v>71</v>
       </c>
       <c r="C2570" s="4">
-        <v>44363</v>
+        <v>44332</v>
       </c>
       <c r="D2570" s="5">
         <v>0.33333333333333298</v>
@@ -83118,13 +83130,13 @@
         <v>86</v>
       </c>
       <c r="I2570">
-        <v>0.05</v>
+        <v>0.45</v>
       </c>
       <c r="J2570" t="s">
         <v>96</v>
       </c>
       <c r="L2570">
-        <v>7.0000000000000007E-2</v>
+        <v>0.46</v>
       </c>
       <c r="M2570" t="s">
         <v>13</v>
@@ -83138,31 +83150,28 @@
         <v>71</v>
       </c>
       <c r="C2571" s="4">
-        <v>44363</v>
+        <v>44332</v>
       </c>
       <c r="D2571" s="5">
-        <v>0.33333333333333298</v>
+        <v>0.34375</v>
       </c>
       <c r="H2571" t="s">
         <v>86</v>
       </c>
       <c r="I2571">
-        <v>0.02</v>
+        <v>0.08</v>
       </c>
       <c r="J2571" t="s">
         <v>96</v>
       </c>
-      <c r="K2571">
-        <v>0.01</v>
-      </c>
       <c r="L2571">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="M2571" t="s">
         <v>13</v>
       </c>
       <c r="N2571" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2572" spans="2:14" x14ac:dyDescent="0.25">
@@ -83178,17 +83187,14 @@
       <c r="H2572" t="s">
         <v>86</v>
       </c>
-      <c r="I2572" t="s">
-        <v>74</v>
+      <c r="I2572">
+        <v>0.05</v>
       </c>
       <c r="J2572" t="s">
         <v>96</v>
       </c>
-      <c r="K2572">
-        <v>0.1</v>
-      </c>
       <c r="L2572">
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M2572" t="s">
         <v>13</v>
@@ -83202,22 +83208,31 @@
         <v>71</v>
       </c>
       <c r="C2573" s="4">
-        <v>44422</v>
+        <v>44363</v>
       </c>
       <c r="D2573" s="5">
-        <v>0.3354166666666667</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="H2573" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I2573">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="J2573" t="s">
         <v>96</v>
       </c>
+      <c r="K2573">
+        <v>0.01</v>
+      </c>
       <c r="L2573">
-        <v>9.4999999999999998E-3</v>
+        <v>0.03</v>
+      </c>
+      <c r="M2573" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2573" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2574" spans="2:14" x14ac:dyDescent="0.25">
@@ -83225,22 +83240,31 @@
         <v>71</v>
       </c>
       <c r="C2574" s="4">
-        <v>44360</v>
+        <v>44363</v>
       </c>
       <c r="D2574" s="5">
-        <v>0.27083333333333298</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="H2574" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2574">
+        <v>86</v>
+      </c>
+      <c r="I2574" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2574" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2574">
+        <v>0.1</v>
+      </c>
+      <c r="L2574">
         <v>0.11</v>
       </c>
-      <c r="J2574" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2574">
-        <v>0.12</v>
+      <c r="M2574" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2574" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2575" spans="2:14" x14ac:dyDescent="0.25">
@@ -83248,22 +83272,22 @@
         <v>71</v>
       </c>
       <c r="C2575" s="4">
-        <v>44360</v>
+        <v>44422</v>
       </c>
       <c r="D2575" s="5">
-        <v>0.27222222222222198</v>
+        <v>0.3354166666666667</v>
       </c>
       <c r="H2575" t="s">
         <v>68</v>
       </c>
       <c r="I2575">
-        <v>0.1</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="J2575" t="s">
         <v>96</v>
       </c>
       <c r="L2575">
-        <v>0.09</v>
+        <v>9.4999999999999998E-3</v>
       </c>
     </row>
     <row r="2576" spans="2:14" x14ac:dyDescent="0.25">
@@ -83274,22 +83298,22 @@
         <v>44360</v>
       </c>
       <c r="D2576" s="5">
-        <v>0.30555555555555602</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="H2576" t="s">
         <v>68</v>
       </c>
       <c r="I2576">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="J2576" t="s">
         <v>96</v>
       </c>
-      <c r="L2576" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2577" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L2576">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="2577" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2577" t="s">
         <v>71</v>
       </c>
@@ -83297,22 +83321,22 @@
         <v>44360</v>
       </c>
       <c r="D2577" s="5">
-        <v>0.33333333333333298</v>
+        <v>0.27222222222222198</v>
       </c>
       <c r="H2577" t="s">
         <v>68</v>
       </c>
       <c r="I2577">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J2577" t="s">
         <v>96</v>
       </c>
       <c r="L2577">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="2578" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="2578" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2578" t="s">
         <v>71</v>
       </c>
@@ -83320,22 +83344,22 @@
         <v>44360</v>
       </c>
       <c r="D2578" s="5">
-        <v>0.3354166666666667</v>
+        <v>0.30555555555555602</v>
       </c>
       <c r="H2578" t="s">
         <v>68</v>
       </c>
       <c r="I2578">
-        <v>7.0000000000000007E-2</v>
+        <v>0.15</v>
       </c>
       <c r="J2578" t="s">
         <v>96</v>
       </c>
-      <c r="L2578">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="2579" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L2578" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2579" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2579" t="s">
         <v>71</v>
       </c>
@@ -83343,22 +83367,22 @@
         <v>44360</v>
       </c>
       <c r="D2579" s="5">
-        <v>0.3354166666666667</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="H2579" t="s">
         <v>68</v>
       </c>
       <c r="I2579">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J2579" t="s">
         <v>96</v>
       </c>
       <c r="L2579">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="2580" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="2580" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2580" t="s">
         <v>71</v>
       </c>
@@ -83372,16 +83396,16 @@
         <v>68</v>
       </c>
       <c r="I2580">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J2580" t="s">
         <v>96</v>
       </c>
       <c r="L2580">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="2581" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2581" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2581" t="s">
         <v>71</v>
       </c>
@@ -83395,16 +83419,16 @@
         <v>68</v>
       </c>
       <c r="I2581">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="J2581" t="s">
         <v>96</v>
       </c>
       <c r="L2581">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="2582" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="2582" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2582" t="s">
         <v>71</v>
       </c>
@@ -83412,22 +83436,22 @@
         <v>44360</v>
       </c>
       <c r="D2582" s="5">
-        <v>0.37847222222222199</v>
+        <v>0.3354166666666667</v>
       </c>
       <c r="H2582" t="s">
         <v>68</v>
       </c>
       <c r="I2582">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="J2582" t="s">
         <v>96</v>
       </c>
       <c r="L2582">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="2583" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2583" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2583" t="s">
         <v>71</v>
       </c>
@@ -83435,22 +83459,22 @@
         <v>44360</v>
       </c>
       <c r="D2583" s="5">
-        <v>0.39583333333333298</v>
+        <v>0.3354166666666667</v>
       </c>
       <c r="H2583" t="s">
         <v>68</v>
       </c>
       <c r="I2583">
-        <v>0.08</v>
+        <v>0.4</v>
       </c>
       <c r="J2583" t="s">
         <v>96</v>
       </c>
       <c r="L2583">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="2584" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="2584" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2584" t="s">
         <v>71</v>
       </c>
@@ -83458,7 +83482,7 @@
         <v>44360</v>
       </c>
       <c r="D2584" s="5">
-        <v>0.42013888888888901</v>
+        <v>0.37847222222222199</v>
       </c>
       <c r="H2584" t="s">
         <v>68</v>
@@ -83470,50 +83494,56 @@
         <v>96</v>
       </c>
       <c r="L2584">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="2585" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="2585" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2585" t="s">
         <v>71</v>
       </c>
       <c r="C2585" s="4">
-        <v>44389</v>
+        <v>44360</v>
+      </c>
+      <c r="D2585" s="5">
+        <v>0.39583333333333298</v>
       </c>
       <c r="H2585" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I2585">
-        <v>7.2</v>
+        <v>0.08</v>
       </c>
       <c r="J2585" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2585">
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="2586" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="2586" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2586" t="s">
         <v>71</v>
       </c>
       <c r="C2586" s="4">
-        <v>44389</v>
+        <v>44360</v>
+      </c>
+      <c r="D2586" s="5">
+        <v>0.42013888888888901</v>
       </c>
       <c r="H2586" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I2586">
-        <v>6.1</v>
+        <v>0.2</v>
       </c>
       <c r="J2586" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2586">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="2587" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="2587" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2587" t="s">
         <v>71</v>
       </c>
@@ -83524,149 +83554,113 @@
         <v>66</v>
       </c>
       <c r="I2587">
-        <v>6.85</v>
+        <v>7.2</v>
       </c>
       <c r="J2587" t="s">
         <v>67</v>
       </c>
       <c r="L2587">
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="2588" spans="2:14" x14ac:dyDescent="0.25">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="2588" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2588" t="s">
         <v>71</v>
       </c>
       <c r="C2588" s="4">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="H2588" t="s">
         <v>66</v>
       </c>
       <c r="I2588">
-        <v>7.2</v>
+        <v>6.1</v>
       </c>
       <c r="J2588" t="s">
         <v>67</v>
       </c>
       <c r="L2588">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="2589" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2589" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2589" s="4">
+        <v>44391</v>
+      </c>
+      <c r="H2589" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2589">
+        <v>6.85</v>
+      </c>
+      <c r="J2589" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2589">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="2590" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2590" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2590" s="4">
+        <v>44392</v>
+      </c>
+      <c r="H2590" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2590">
+        <v>7.2</v>
+      </c>
+      <c r="J2590" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2590">
         <v>9</v>
       </c>
     </row>
-    <row r="2589" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2589" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2589" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2589" s="5">
-        <v>0.27083333333333298</v>
-      </c>
-      <c r="H2589" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2589">
-        <v>0.9</v>
-      </c>
-      <c r="J2589" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2589">
-        <v>0.8</v>
-      </c>
-      <c r="M2589" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2589" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2590" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2590" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2590" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2590" s="5">
-        <v>0.27777777777777801</v>
-      </c>
-      <c r="H2590" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2590">
-        <v>0.3</v>
-      </c>
-      <c r="J2590" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2590">
-        <v>0.3</v>
-      </c>
-      <c r="M2590" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2590" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2591" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2591" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2591" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2591" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2591" s="5">
-        <v>0.28819444444444398</v>
+        <v>44393</v>
       </c>
       <c r="H2591" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="I2591">
-        <v>0.3</v>
+        <v>6.15</v>
       </c>
       <c r="J2591" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="L2591">
-        <v>0.45</v>
-      </c>
-      <c r="M2591" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2591" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2592" spans="2:14" x14ac:dyDescent="0.25">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="2592" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2592" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2592" s="4">
-        <v>44332</v>
-      </c>
-      <c r="D2592" s="5">
-        <v>0.30208333333333298</v>
+        <v>44394</v>
       </c>
       <c r="H2592" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="I2592">
-        <v>0.82</v>
+        <v>6.15</v>
       </c>
       <c r="J2592" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="L2592">
-        <v>0.8</v>
-      </c>
-      <c r="M2592" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2592" t="s">
-        <v>113</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="2593" spans="2:14" x14ac:dyDescent="0.25">
@@ -83677,25 +83671,25 @@
         <v>44332</v>
       </c>
       <c r="D2593" s="5">
-        <v>0.31944444444444398</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="H2593" t="s">
         <v>86</v>
       </c>
       <c r="I2593">
-        <v>0.15</v>
+        <v>0.9</v>
       </c>
       <c r="J2593" t="s">
         <v>96</v>
       </c>
       <c r="L2593">
-        <v>0.12</v>
+        <v>0.8</v>
       </c>
       <c r="M2593" t="s">
         <v>13</v>
       </c>
       <c r="N2593" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2594" spans="2:14" x14ac:dyDescent="0.25">
@@ -83706,25 +83700,25 @@
         <v>44332</v>
       </c>
       <c r="D2594" s="5">
-        <v>0.32638888888888901</v>
+        <v>0.27777777777777801</v>
       </c>
       <c r="H2594" t="s">
         <v>86</v>
       </c>
       <c r="I2594">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
       <c r="J2594" t="s">
         <v>96</v>
       </c>
       <c r="L2594">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="M2594" t="s">
         <v>13</v>
       </c>
       <c r="N2594" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2595" spans="2:14" x14ac:dyDescent="0.25">
@@ -83732,19 +83726,28 @@
         <v>73</v>
       </c>
       <c r="C2595" s="4">
-        <v>44360</v>
+        <v>44332</v>
+      </c>
+      <c r="D2595" s="5">
+        <v>0.28819444444444398</v>
       </c>
       <c r="H2595" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I2595">
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="J2595" t="s">
         <v>96</v>
       </c>
       <c r="L2595">
-        <v>0.11</v>
+        <v>0.45</v>
+      </c>
+      <c r="M2595" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2595" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2596" spans="2:14" x14ac:dyDescent="0.25">
@@ -83752,19 +83755,28 @@
         <v>73</v>
       </c>
       <c r="C2596" s="4">
-        <v>44360</v>
+        <v>44332</v>
+      </c>
+      <c r="D2596" s="5">
+        <v>0.30208333333333298</v>
       </c>
       <c r="H2596" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I2596">
-        <v>0.09</v>
+        <v>0.82</v>
       </c>
       <c r="J2596" t="s">
         <v>96</v>
       </c>
       <c r="L2596">
-        <v>0.1</v>
+        <v>0.8</v>
+      </c>
+      <c r="M2596" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2596" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2597" spans="2:14" x14ac:dyDescent="0.25">
@@ -83772,19 +83784,28 @@
         <v>73</v>
       </c>
       <c r="C2597" s="4">
-        <v>44360</v>
+        <v>44332</v>
+      </c>
+      <c r="D2597" s="5">
+        <v>0.31944444444444398</v>
       </c>
       <c r="H2597" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I2597">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J2597" t="s">
         <v>96</v>
       </c>
       <c r="L2597">
-        <v>0.15</v>
+        <v>0.12</v>
+      </c>
+      <c r="M2597" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2597" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2598" spans="2:14" x14ac:dyDescent="0.25">
@@ -83792,19 +83813,28 @@
         <v>73</v>
       </c>
       <c r="C2598" s="4">
-        <v>44360</v>
+        <v>44332</v>
+      </c>
+      <c r="D2598" s="5">
+        <v>0.32638888888888901</v>
       </c>
       <c r="H2598" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I2598">
-        <v>0.08</v>
+        <v>0.38</v>
       </c>
       <c r="J2598" t="s">
         <v>96</v>
       </c>
       <c r="L2598">
-        <v>7.0000000000000007E-2</v>
+        <v>0.34</v>
+      </c>
+      <c r="M2598" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2598" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2599" spans="2:14" x14ac:dyDescent="0.25">
@@ -83818,13 +83848,13 @@
         <v>68</v>
       </c>
       <c r="I2599">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J2599" t="s">
         <v>96</v>
       </c>
       <c r="L2599">
-        <v>7.0000000000000007E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="2600" spans="2:14" x14ac:dyDescent="0.25">
@@ -83832,19 +83862,19 @@
         <v>73</v>
       </c>
       <c r="C2600" s="4">
-        <v>44361</v>
+        <v>44360</v>
       </c>
       <c r="H2600" t="s">
         <v>68</v>
       </c>
       <c r="I2600">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="J2600" t="s">
         <v>96</v>
       </c>
       <c r="L2600">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="2601" spans="2:14" x14ac:dyDescent="0.25">
@@ -83852,19 +83882,19 @@
         <v>73</v>
       </c>
       <c r="C2601" s="4">
-        <v>44362</v>
+        <v>44360</v>
       </c>
       <c r="H2601" t="s">
         <v>68</v>
       </c>
       <c r="I2601">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="J2601" t="s">
         <v>96</v>
       </c>
       <c r="L2601">
-        <v>7.0000000000000007E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="2602" spans="2:14" x14ac:dyDescent="0.25">
@@ -83872,19 +83902,19 @@
         <v>73</v>
       </c>
       <c r="C2602" s="4">
-        <v>44363</v>
+        <v>44360</v>
       </c>
       <c r="H2602" t="s">
         <v>68</v>
       </c>
       <c r="I2602">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="J2602" t="s">
         <v>96</v>
       </c>
       <c r="L2602">
-        <v>5.0999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="2603" spans="2:14" x14ac:dyDescent="0.25">
@@ -83892,19 +83922,19 @@
         <v>73</v>
       </c>
       <c r="C2603" s="4">
-        <v>44364</v>
+        <v>44360</v>
       </c>
       <c r="H2603" t="s">
         <v>68</v>
       </c>
       <c r="I2603">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J2603" t="s">
         <v>96</v>
       </c>
       <c r="L2603">
-        <v>0.21</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="2604" spans="2:14" x14ac:dyDescent="0.25">
@@ -84007,7 +84037,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="2609" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2609" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2609" t="s">
         <v>73</v>
       </c>
@@ -84027,7 +84057,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="2610" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2610" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2610" t="s">
         <v>73</v>
       </c>
@@ -84038,16 +84068,16 @@
         <v>68</v>
       </c>
       <c r="I2610">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="J2610" t="s">
         <v>96</v>
       </c>
       <c r="L2610">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="2611" spans="2:14" x14ac:dyDescent="0.25">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="2611" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2611" t="s">
         <v>73</v>
       </c>
@@ -84058,16 +84088,16 @@
         <v>68</v>
       </c>
       <c r="I2611">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
       <c r="J2611" t="s">
         <v>96</v>
       </c>
       <c r="L2611">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="2612" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="2612" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2612" t="s">
         <v>73</v>
       </c>
@@ -84087,7 +84117,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="2613" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2613" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2613" t="s">
         <v>73</v>
       </c>
@@ -84107,7 +84137,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="2614" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2614" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2614" t="s">
         <v>73</v>
       </c>
@@ -84118,16 +84148,16 @@
         <v>68</v>
       </c>
       <c r="I2614">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="J2614" t="s">
         <v>96</v>
       </c>
       <c r="L2614">
-        <v>5.0999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="2615" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="2615" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2615" t="s">
         <v>73</v>
       </c>
@@ -84138,289 +84168,253 @@
         <v>68</v>
       </c>
       <c r="I2615">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="J2615" t="s">
         <v>96</v>
       </c>
       <c r="L2615">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="2616" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="2616" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2616" t="s">
         <v>73</v>
       </c>
       <c r="C2616" s="4">
-        <v>44239</v>
+        <v>44361</v>
       </c>
       <c r="H2616" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2616" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="I2616">
+        <v>0.08</v>
       </c>
       <c r="J2616" t="s">
         <v>96</v>
       </c>
-      <c r="L2616" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2617" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L2616">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="2617" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2617" t="s">
         <v>73</v>
       </c>
       <c r="C2617" s="4">
-        <v>44243</v>
+        <v>44362</v>
       </c>
       <c r="H2617" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="I2617">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J2617" t="s">
         <v>96</v>
       </c>
       <c r="L2617">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="2618" spans="2:14" x14ac:dyDescent="0.25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="2618" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2618" t="s">
         <v>73</v>
       </c>
       <c r="C2618" s="4">
-        <v>44240</v>
+        <v>44363</v>
       </c>
       <c r="H2618" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2618" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="I2618">
+        <v>0.05</v>
       </c>
       <c r="J2618" t="s">
         <v>96</v>
       </c>
       <c r="L2618">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="2619" spans="2:14" x14ac:dyDescent="0.25">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="2619" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2619" t="s">
         <v>73</v>
       </c>
       <c r="C2619" s="4">
-        <v>44241</v>
+        <v>44364</v>
       </c>
       <c r="H2619" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="I2619">
-        <v>0.04</v>
+        <v>0.2</v>
       </c>
       <c r="J2619" t="s">
         <v>96</v>
       </c>
       <c r="L2619">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="2620" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="2620" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2620" t="s">
         <v>73</v>
       </c>
       <c r="C2620" s="4">
-        <v>44242</v>
+        <v>44239</v>
       </c>
       <c r="H2620" t="s">
         <v>91</v>
       </c>
-      <c r="I2620">
-        <v>0.04</v>
+      <c r="I2620" t="s">
+        <v>74</v>
       </c>
       <c r="J2620" t="s">
         <v>96</v>
       </c>
-      <c r="L2620">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="2621" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L2620" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2621" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2621" t="s">
         <v>73</v>
       </c>
       <c r="C2621" s="4">
-        <v>44244</v>
+        <v>44243</v>
       </c>
       <c r="H2621" t="s">
         <v>91</v>
       </c>
       <c r="I2621">
-        <v>4.5999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J2621" t="s">
         <v>96</v>
       </c>
       <c r="L2621">
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="2622" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="2622" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2622" t="s">
         <v>73</v>
       </c>
       <c r="C2622" s="4">
-        <v>44245</v>
+        <v>44240</v>
       </c>
       <c r="H2622" t="s">
         <v>91</v>
       </c>
-      <c r="I2622">
-        <v>5.0999999999999997E-2</v>
+      <c r="I2622" t="s">
+        <v>74</v>
       </c>
       <c r="J2622" t="s">
         <v>96</v>
       </c>
       <c r="L2622">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="2623" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="2623" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2623" t="s">
         <v>73</v>
       </c>
       <c r="C2623" s="4">
-        <v>44246</v>
+        <v>44241</v>
       </c>
       <c r="H2623" t="s">
         <v>91</v>
       </c>
       <c r="I2623">
-        <v>4.5499999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J2623" t="s">
         <v>96</v>
       </c>
       <c r="L2623">
-        <v>5.45E-2</v>
-      </c>
-    </row>
-    <row r="2624" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2624" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2624" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C2624" s="4">
-        <v>44360</v>
-      </c>
-      <c r="D2624" s="5">
-        <v>0.27986111111111101</v>
+        <v>44242</v>
       </c>
       <c r="H2624" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="I2624">
-        <v>7.21</v>
+        <v>0.04</v>
       </c>
       <c r="J2624" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2624">
-        <v>7</v>
-      </c>
-      <c r="M2624" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2624" t="s">
-        <v>124</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="2625" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2625" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C2625" s="4">
-        <v>44360</v>
-      </c>
-      <c r="D2625" s="5">
-        <v>0.30416666666666697</v>
+        <v>44244</v>
       </c>
       <c r="H2625" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="I2625">
-        <v>7.38</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J2625" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2625">
-        <v>7</v>
-      </c>
-      <c r="M2625" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2625" t="s">
-        <v>125</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="2626" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2626" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C2626" s="4">
-        <v>44360</v>
-      </c>
-      <c r="D2626" s="5">
-        <v>0.33124999999999999</v>
+        <v>44245</v>
       </c>
       <c r="H2626" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="I2626">
-        <v>7.39</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J2626" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2626">
-        <v>7</v>
-      </c>
-      <c r="M2626" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2626" t="s">
-        <v>126</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="2627" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2627" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C2627" s="4">
-        <v>44360</v>
-      </c>
-      <c r="D2627" s="5">
-        <v>0.33472222222222198</v>
+        <v>44246</v>
       </c>
       <c r="H2627" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="I2627">
-        <v>7.23</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="J2627" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L2627">
-        <v>7</v>
-      </c>
-      <c r="M2627" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2627" t="s">
-        <v>127</v>
+        <v>5.45E-2</v>
       </c>
     </row>
     <row r="2628" spans="2:14" x14ac:dyDescent="0.25">
@@ -84431,13 +84425,13 @@
         <v>44360</v>
       </c>
       <c r="D2628" s="5">
-        <v>0.37847222222222199</v>
+        <v>0.27986111111111101</v>
       </c>
       <c r="H2628" t="s">
         <v>66</v>
       </c>
       <c r="I2628">
-        <v>6.92</v>
+        <v>7.21</v>
       </c>
       <c r="J2628" t="s">
         <v>67</v>
@@ -84449,7 +84443,7 @@
         <v>13</v>
       </c>
       <c r="N2628" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2629" spans="2:14" x14ac:dyDescent="0.25">
@@ -84460,13 +84454,13 @@
         <v>44360</v>
       </c>
       <c r="D2629" s="5">
-        <v>0.38541666666666702</v>
+        <v>0.30416666666666697</v>
       </c>
       <c r="H2629" t="s">
         <v>66</v>
       </c>
       <c r="I2629">
-        <v>7.23</v>
+        <v>7.38</v>
       </c>
       <c r="J2629" t="s">
         <v>67</v>
@@ -84478,7 +84472,7 @@
         <v>13</v>
       </c>
       <c r="N2629" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2630" spans="2:14" x14ac:dyDescent="0.25">
@@ -84486,25 +84480,28 @@
         <v>101</v>
       </c>
       <c r="C2630" s="4">
-        <v>44451</v>
+        <v>44360</v>
       </c>
       <c r="D2630" s="5">
-        <v>0.28749999999999998</v>
+        <v>0.33124999999999999</v>
       </c>
       <c r="H2630" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2630">
-        <v>1010</v>
+        <v>7.39</v>
       </c>
       <c r="J2630" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2630">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="M2630" t="s">
         <v>13</v>
+      </c>
+      <c r="N2630" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2631" spans="2:14" x14ac:dyDescent="0.25">
@@ -84512,25 +84509,28 @@
         <v>101</v>
       </c>
       <c r="C2631" s="4">
-        <v>44451</v>
+        <v>44360</v>
       </c>
       <c r="D2631" s="5">
-        <v>0.30208333333333298</v>
+        <v>0.33472222222222198</v>
       </c>
       <c r="H2631" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2631">
-        <v>950</v>
+        <v>7.23</v>
       </c>
       <c r="J2631" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2631">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="M2631" t="s">
         <v>13</v>
+      </c>
+      <c r="N2631" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="2632" spans="2:14" x14ac:dyDescent="0.25">
@@ -84538,25 +84538,28 @@
         <v>101</v>
       </c>
       <c r="C2632" s="4">
-        <v>44451</v>
+        <v>44362</v>
       </c>
       <c r="D2632" s="5">
-        <v>0.31458333333333299</v>
+        <v>0.33472222222222198</v>
       </c>
       <c r="H2632" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2632">
-        <v>1001</v>
+        <v>7.23</v>
       </c>
       <c r="J2632" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2632">
-        <v>1000</v>
+        <v>7.02</v>
       </c>
       <c r="M2632" t="s">
         <v>13</v>
+      </c>
+      <c r="N2632" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2633" spans="2:14" x14ac:dyDescent="0.25">
@@ -84564,25 +84567,28 @@
         <v>101</v>
       </c>
       <c r="C2633" s="4">
-        <v>44451</v>
+        <v>44363</v>
       </c>
       <c r="D2633" s="5">
-        <v>0.31944444444444398</v>
+        <v>0.33472222222222198</v>
       </c>
       <c r="H2633" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2633">
-        <v>1040</v>
+        <v>7.02</v>
       </c>
       <c r="J2633" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2633">
-        <v>1000</v>
+        <v>7.02</v>
       </c>
       <c r="M2633" t="s">
         <v>13</v>
+      </c>
+      <c r="N2633" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2634" spans="2:14" x14ac:dyDescent="0.25">
@@ -84590,25 +84596,28 @@
         <v>101</v>
       </c>
       <c r="C2634" s="4">
-        <v>44451</v>
+        <v>44364</v>
       </c>
       <c r="D2634" s="5">
-        <v>0.34027777777777801</v>
+        <v>0.33472222222222198</v>
       </c>
       <c r="H2634" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2634">
-        <v>1100</v>
+        <v>7.056</v>
       </c>
       <c r="J2634" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2634">
-        <v>1000</v>
+        <v>7.02</v>
       </c>
       <c r="M2634" t="s">
         <v>13</v>
+      </c>
+      <c r="N2634" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2635" spans="2:14" x14ac:dyDescent="0.25">
@@ -84616,25 +84625,28 @@
         <v>101</v>
       </c>
       <c r="C2635" s="4">
-        <v>44451</v>
+        <v>44360</v>
       </c>
       <c r="D2635" s="5">
-        <v>0.34027777777777801</v>
+        <v>0.37847222222222199</v>
       </c>
       <c r="H2635" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2635">
-        <v>165</v>
+        <v>6.92</v>
       </c>
       <c r="J2635" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2635">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="M2635" t="s">
         <v>13</v>
+      </c>
+      <c r="N2635" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2636" spans="2:14" x14ac:dyDescent="0.25">
@@ -84642,25 +84654,28 @@
         <v>101</v>
       </c>
       <c r="C2636" s="4">
-        <v>44451</v>
+        <v>44360</v>
       </c>
       <c r="D2636" s="5">
-        <v>0.34722222222222199</v>
+        <v>0.38541666666666702</v>
       </c>
       <c r="H2636" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I2636">
-        <v>750</v>
+        <v>7.23</v>
       </c>
       <c r="J2636" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="L2636">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="M2636" t="s">
         <v>13</v>
+      </c>
+      <c r="N2636" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="2637" spans="2:14" x14ac:dyDescent="0.25">
@@ -84671,13 +84686,13 @@
         <v>44451</v>
       </c>
       <c r="D2637" s="5">
-        <v>0.35</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="H2637" t="s">
         <v>90</v>
       </c>
       <c r="I2637">
-        <v>999</v>
+        <v>1010</v>
       </c>
       <c r="J2637" t="s">
         <v>98</v>
@@ -84697,13 +84712,13 @@
         <v>44451</v>
       </c>
       <c r="D2638" s="5">
-        <v>0.358333333333333</v>
+        <v>0.30208333333333298</v>
       </c>
       <c r="H2638" t="s">
         <v>90</v>
       </c>
       <c r="I2638">
-        <v>980</v>
+        <v>950</v>
       </c>
       <c r="J2638" t="s">
         <v>98</v>
@@ -84723,13 +84738,13 @@
         <v>44451</v>
       </c>
       <c r="D2639" s="5">
-        <v>0.38402777777777802</v>
+        <v>0.31458333333333299</v>
       </c>
       <c r="H2639" t="s">
         <v>90</v>
       </c>
       <c r="I2639">
-        <v>420</v>
+        <v>1001</v>
       </c>
       <c r="J2639" t="s">
         <v>98</v>
@@ -84741,10 +84756,374 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2640" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2640" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2640" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2640" s="5">
+        <v>0.31944444444444398</v>
+      </c>
+      <c r="H2640" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2640">
+        <v>1040</v>
+      </c>
+      <c r="J2640" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2640">
+        <v>1000</v>
+      </c>
+      <c r="M2640" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2641" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2641" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2641" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2641" s="5">
+        <v>0.34027777777777801</v>
+      </c>
+      <c r="H2641" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2641">
+        <v>1100</v>
+      </c>
+      <c r="J2641" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2641">
+        <v>1000</v>
+      </c>
+      <c r="M2641" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2642" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2642" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2642" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2642" s="5">
+        <v>0.34027777777777801</v>
+      </c>
+      <c r="H2642" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2642">
+        <v>165</v>
+      </c>
+      <c r="J2642" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2642">
+        <v>100</v>
+      </c>
+      <c r="M2642" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2643" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2643" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2643" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2643" s="5">
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="H2643" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2643">
+        <v>750</v>
+      </c>
+      <c r="J2643" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2643">
+        <v>1000</v>
+      </c>
+      <c r="M2643" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2644" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2644" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2644" s="4">
+        <v>44420</v>
+      </c>
+      <c r="D2644" s="5">
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="H2644" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2644">
+        <v>986.2</v>
+      </c>
+      <c r="J2644" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2644">
+        <v>1000</v>
+      </c>
+      <c r="M2644" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2645" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2645" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2645" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2645" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="H2645" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2645">
+        <v>999</v>
+      </c>
+      <c r="J2645" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2645">
+        <v>1000</v>
+      </c>
+      <c r="M2645" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2646" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2646" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2646" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2646" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2646" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2646">
+        <v>980</v>
+      </c>
+      <c r="J2646" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2646">
+        <v>1000</v>
+      </c>
+      <c r="M2646" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2647" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2647" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2647" s="4">
+        <v>44451</v>
+      </c>
+      <c r="D2647" s="5">
+        <v>0.38402777777777802</v>
+      </c>
+      <c r="H2647" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2647">
+        <v>420</v>
+      </c>
+      <c r="J2647" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2647">
+        <v>1000</v>
+      </c>
+      <c r="M2647" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2648" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2648" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2648" s="4">
+        <v>44481</v>
+      </c>
+      <c r="D2648" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2648" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2648">
+        <v>102</v>
+      </c>
+      <c r="J2648" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2648">
+        <v>100</v>
+      </c>
+      <c r="M2648" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2649" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2649" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2649" s="4">
+        <v>44482</v>
+      </c>
+      <c r="D2649" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2649" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2649">
+        <v>105.36</v>
+      </c>
+      <c r="J2649" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2649">
+        <v>100.6</v>
+      </c>
+      <c r="M2649" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2650" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2650" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2650" s="4">
+        <v>44483</v>
+      </c>
+      <c r="D2650" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2650" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2650">
+        <v>75</v>
+      </c>
+      <c r="J2650" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2650">
+        <v>99.8</v>
+      </c>
+      <c r="M2650" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2651" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2651" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2651" s="4">
+        <v>44484</v>
+      </c>
+      <c r="D2651" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2651" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2651">
+        <v>26</v>
+      </c>
+      <c r="J2651" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2651">
+        <v>22</v>
+      </c>
+      <c r="M2651" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2652" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2652" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2652" s="4">
+        <v>44484</v>
+      </c>
+      <c r="D2652" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2652" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2652">
+        <v>6.4</v>
+      </c>
+      <c r="J2652" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2652">
+        <v>6</v>
+      </c>
+      <c r="M2652" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2653" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2653" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2653" s="4">
+        <v>44485</v>
+      </c>
+      <c r="D2653" s="5">
+        <v>0.358333333333333</v>
+      </c>
+      <c r="H2653" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2653">
+        <v>6.2</v>
+      </c>
+      <c r="J2653" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2653">
+        <v>6</v>
+      </c>
+      <c r="M2653" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2641">
-    <sortCondition ref="B2:B2641"/>
-    <sortCondition ref="H2:H2641"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2649">
+    <sortCondition ref="B2:B2649"/>
+    <sortCondition ref="H2:H2649"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update parameter mapping with removed columns, update results example file with wqx columns and fix checks
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleResults.xlsx
+++ b/inst/extdata/ExampleResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA845B59-DFA3-44BD-B103-00ACC15942F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B333CB1-DF5A-459C-A543-F9D9326D0E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="30885" yWindow="1095" windowWidth="23595" windowHeight="13380" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16083" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16086" uniqueCount="142">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -496,6 +496,15 @@
   <si>
     <t>pH-6-17-5</t>
   </si>
+  <si>
+    <t>Sample Collection Method ID</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Result Comment</t>
+  </si>
 </sst>
 </file>
 
@@ -578,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,6 +610,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -918,13 +930,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N2653"/>
+  <dimension ref="A1:Q2653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E957" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I968" sqref="I968"/>
+      <selection pane="bottomRight" activeCell="N963" sqref="N963"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,9 +951,12 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -984,8 +999,17 @@
       <c r="N1" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +1041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1049,7 +1073,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1113,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1177,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1305,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1337,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1401,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
update activity type inputs in results file and output for tabMWRwqx, change order of activity id in tabMWRwqx, add warning for no UQL or MDL
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleResults.xlsx
+++ b/inst/extdata/ExampleResults.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B333CB1-DF5A-459C-A543-F9D9326D0E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD2931-E460-4182-A1AF-B481EDFDFE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="1095" windowWidth="23595" windowHeight="13380" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="2355" yWindow="915" windowWidth="21600" windowHeight="11325" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$N$2500</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$Q$2653</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -383,9 +383,6 @@
     <t>cfu/100ml</t>
   </si>
   <si>
-    <t>Quality Control Field Calibration Check</t>
-  </si>
-  <si>
     <t>K16452-MB1</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   <si>
     <t>Result Comment</t>
   </si>
+  <si>
+    <t>Quality Control-Calibration Check</t>
+  </si>
 </sst>
 </file>
 
@@ -587,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,9 +610,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,10 +930,10 @@
   <dimension ref="A1:Q2653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E957" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2620" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N963" sqref="N963"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,14 +996,14 @@
       <c r="N1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -82579,7 +82576,7 @@
         <v>96</v>
       </c>
       <c r="N2545" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2546" spans="2:14" x14ac:dyDescent="0.25">
@@ -82599,7 +82596,7 @@
         <v>96</v>
       </c>
       <c r="N2546" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2547" spans="2:14" x14ac:dyDescent="0.25">
@@ -82619,7 +82616,7 @@
         <v>96</v>
       </c>
       <c r="N2547" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2548" spans="2:14" x14ac:dyDescent="0.25">
@@ -82639,7 +82636,7 @@
         <v>96</v>
       </c>
       <c r="N2548" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2549" spans="2:14" x14ac:dyDescent="0.25">
@@ -82659,7 +82656,7 @@
         <v>96</v>
       </c>
       <c r="N2549" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2550" spans="2:14" x14ac:dyDescent="0.25">
@@ -82679,7 +82676,7 @@
         <v>96</v>
       </c>
       <c r="N2550" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2551" spans="2:14" x14ac:dyDescent="0.25">
@@ -82699,7 +82696,7 @@
         <v>96</v>
       </c>
       <c r="N2551" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2552" spans="2:14" x14ac:dyDescent="0.25">
@@ -82719,7 +82716,7 @@
         <v>96</v>
       </c>
       <c r="N2552" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2553" spans="2:14" x14ac:dyDescent="0.25">
@@ -82833,7 +82830,7 @@
         <v>13</v>
       </c>
       <c r="N2558" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2559" spans="2:14" x14ac:dyDescent="0.25">
@@ -82859,7 +82856,7 @@
         <v>13</v>
       </c>
       <c r="N2559" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2560" spans="2:14" x14ac:dyDescent="0.25">
@@ -82885,7 +82882,7 @@
         <v>13</v>
       </c>
       <c r="N2560" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2561" spans="2:14" x14ac:dyDescent="0.25">
@@ -82911,7 +82908,7 @@
         <v>13</v>
       </c>
       <c r="N2561" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2562" spans="2:14" x14ac:dyDescent="0.25">
@@ -82937,7 +82934,7 @@
         <v>13</v>
       </c>
       <c r="N2562" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2563" spans="2:14" x14ac:dyDescent="0.25">
@@ -82963,7 +82960,7 @@
         <v>13</v>
       </c>
       <c r="N2563" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2564" spans="2:14" x14ac:dyDescent="0.25">
@@ -82992,7 +82989,7 @@
         <v>13</v>
       </c>
       <c r="N2564" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2565" spans="2:14" x14ac:dyDescent="0.25">
@@ -83021,7 +83018,7 @@
         <v>13</v>
       </c>
       <c r="N2565" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2566" spans="2:14" x14ac:dyDescent="0.25">
@@ -83050,7 +83047,7 @@
         <v>13</v>
       </c>
       <c r="N2566" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2567" spans="2:14" x14ac:dyDescent="0.25">
@@ -83079,7 +83076,7 @@
         <v>13</v>
       </c>
       <c r="N2567" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2568" spans="2:14" x14ac:dyDescent="0.25">
@@ -83108,7 +83105,7 @@
         <v>13</v>
       </c>
       <c r="N2568" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2569" spans="2:14" x14ac:dyDescent="0.25">
@@ -83137,7 +83134,7 @@
         <v>13</v>
       </c>
       <c r="N2569" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2570" spans="2:14" x14ac:dyDescent="0.25">
@@ -83166,7 +83163,7 @@
         <v>13</v>
       </c>
       <c r="N2570" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2571" spans="2:14" x14ac:dyDescent="0.25">
@@ -83195,7 +83192,7 @@
         <v>13</v>
       </c>
       <c r="N2571" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2572" spans="2:14" x14ac:dyDescent="0.25">
@@ -83224,7 +83221,7 @@
         <v>13</v>
       </c>
       <c r="N2572" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2573" spans="2:14" x14ac:dyDescent="0.25">
@@ -83256,7 +83253,7 @@
         <v>13</v>
       </c>
       <c r="N2573" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2574" spans="2:14" x14ac:dyDescent="0.25">
@@ -83288,7 +83285,7 @@
         <v>13</v>
       </c>
       <c r="N2574" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2575" spans="2:14" x14ac:dyDescent="0.25">
@@ -83713,7 +83710,7 @@
         <v>13</v>
       </c>
       <c r="N2593" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2594" spans="2:14" x14ac:dyDescent="0.25">
@@ -83742,7 +83739,7 @@
         <v>13</v>
       </c>
       <c r="N2594" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2595" spans="2:14" x14ac:dyDescent="0.25">
@@ -83771,7 +83768,7 @@
         <v>13</v>
       </c>
       <c r="N2595" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2596" spans="2:14" x14ac:dyDescent="0.25">
@@ -83800,7 +83797,7 @@
         <v>13</v>
       </c>
       <c r="N2596" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2597" spans="2:14" x14ac:dyDescent="0.25">
@@ -83829,7 +83826,7 @@
         <v>13</v>
       </c>
       <c r="N2597" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2598" spans="2:14" x14ac:dyDescent="0.25">
@@ -83858,7 +83855,7 @@
         <v>13</v>
       </c>
       <c r="N2598" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2599" spans="2:14" x14ac:dyDescent="0.25">
@@ -84443,7 +84440,7 @@
     </row>
     <row r="2628" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2628" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2628" s="4">
         <v>44360</v>
@@ -84467,12 +84464,12 @@
         <v>13</v>
       </c>
       <c r="N2628" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2629" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2629" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2629" s="4">
         <v>44360</v>
@@ -84496,12 +84493,12 @@
         <v>13</v>
       </c>
       <c r="N2629" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2630" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2630" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2630" s="4">
         <v>44360</v>
@@ -84525,12 +84522,12 @@
         <v>13</v>
       </c>
       <c r="N2630" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2631" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2631" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2631" s="4">
         <v>44360</v>
@@ -84554,12 +84551,12 @@
         <v>13</v>
       </c>
       <c r="N2631" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2632" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2632" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2632" s="4">
         <v>44362</v>
@@ -84583,12 +84580,12 @@
         <v>13</v>
       </c>
       <c r="N2632" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2633" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2633" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2633" s="4">
         <v>44363</v>
@@ -84612,12 +84609,12 @@
         <v>13</v>
       </c>
       <c r="N2633" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2634" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2634" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2634" s="4">
         <v>44364</v>
@@ -84641,12 +84638,12 @@
         <v>13</v>
       </c>
       <c r="N2634" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2635" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2635" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2635" s="4">
         <v>44360</v>
@@ -84670,12 +84667,12 @@
         <v>13</v>
       </c>
       <c r="N2635" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2636" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2636" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2636" s="4">
         <v>44360</v>
@@ -84699,12 +84696,12 @@
         <v>13</v>
       </c>
       <c r="N2636" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2637" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2637" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2637" s="4">
         <v>44451</v>
@@ -84730,7 +84727,7 @@
     </row>
     <row r="2638" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2638" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2638" s="4">
         <v>44451</v>
@@ -84756,7 +84753,7 @@
     </row>
     <row r="2639" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2639" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2639" s="4">
         <v>44451</v>
@@ -84782,7 +84779,7 @@
     </row>
     <row r="2640" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2640" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2640" s="4">
         <v>44451</v>
@@ -84808,7 +84805,7 @@
     </row>
     <row r="2641" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2641" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2641" s="4">
         <v>44451</v>
@@ -84834,7 +84831,7 @@
     </row>
     <row r="2642" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2642" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2642" s="4">
         <v>44451</v>
@@ -84860,7 +84857,7 @@
     </row>
     <row r="2643" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2643" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2643" s="4">
         <v>44451</v>
@@ -84886,7 +84883,7 @@
     </row>
     <row r="2644" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2644" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2644" s="4">
         <v>44420</v>
@@ -84912,7 +84909,7 @@
     </row>
     <row r="2645" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2645" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2645" s="4">
         <v>44451</v>
@@ -84938,7 +84935,7 @@
     </row>
     <row r="2646" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2646" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2646" s="4">
         <v>44451</v>
@@ -84964,7 +84961,7 @@
     </row>
     <row r="2647" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2647" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2647" s="4">
         <v>44451</v>
@@ -84990,7 +84987,7 @@
     </row>
     <row r="2648" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2648" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2648" s="4">
         <v>44481</v>
@@ -85016,7 +85013,7 @@
     </row>
     <row r="2649" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2649" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2649" s="4">
         <v>44482</v>
@@ -85042,7 +85039,7 @@
     </row>
     <row r="2650" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2650" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2650" s="4">
         <v>44483</v>
@@ -85068,7 +85065,7 @@
     </row>
     <row r="2651" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2651" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2651" s="4">
         <v>44484</v>
@@ -85094,7 +85091,7 @@
     </row>
     <row r="2652" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2652" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2652" s="4">
         <v>44484</v>
@@ -85120,7 +85117,7 @@
     </row>
     <row r="2653" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2653" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2653" s="4">
         <v>44485</v>
@@ -85145,6 +85142,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q2653" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2649">
     <sortCondition ref="B2:B2649"/>
     <sortCondition ref="H2:H2649"/>

</xml_diff>